<commit_message>
CN0713: Recursos sin imagenes
</commit_message>
<xml_diff>
--- a/seguimiento/ProduccionDigital/SegDigital_CN_07_13_CO.xlsx
+++ b/seguimiento/ProduccionDigital/SegDigital_CN_07_13_CO.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\CienciasNaturales\seguimiento\ProduccionDigital\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21721" windowHeight="9718"/>
+    <workbookView xWindow="0" yWindow="180" windowWidth="20730" windowHeight="9540"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="66">
   <si>
     <t>Cuaderno de estudio</t>
   </si>
@@ -219,6 +214,12 @@
   </si>
   <si>
     <t>si</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Guía Didáctica</t>
   </si>
 </sst>
 </file>
@@ -298,7 +299,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,8 +324,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -347,13 +354,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -397,11 +430,29 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -677,7 +728,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -685,617 +736,779 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G4" sqref="G4:G26"/>
+      <selection pane="topRight" activeCell="D4" sqref="D4:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.46484375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="1" customWidth="1"/>
-    <col min="5" max="7" width="12" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.06640625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.796875" style="1"/>
+    <col min="1" max="1" width="7.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="1" customWidth="1"/>
+    <col min="6" max="8" width="12" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18" style="1" customWidth="1"/>
+    <col min="10" max="12" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.100000000000001" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" ht="21.15" x14ac:dyDescent="0.45">
+      <c r="C1" s="19"/>
+    </row>
+    <row r="3" spans="1:16" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="M3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="N3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="N3" s="3"/>
       <c r="O3" s="3"/>
-    </row>
-    <row r="4" spans="1:15" ht="15.85" x14ac:dyDescent="0.45">
-      <c r="A4" s="14" t="s">
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:16" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="16">
+      <c r="F5" s="18">
         <v>42094.4375</v>
       </c>
-      <c r="F4" s="16">
+      <c r="G5" s="18">
         <v>42094.447916666664</v>
       </c>
-      <c r="G4" s="16">
+      <c r="H5" s="18">
         <v>42094.458333333336</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="16"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A5" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="9"/>
+      <c r="I5" s="13"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="16"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="L5" s="9"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="18"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="13">
+        <v>42094</v>
+      </c>
+      <c r="J6" s="13">
+        <v>42094</v>
+      </c>
+      <c r="K6" s="13">
+        <v>42094</v>
+      </c>
+      <c r="L6" s="9"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="18"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B7" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="C7" s="11"/>
+      <c r="D7" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="16"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A7" s="10" t="s">
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="13">
+        <v>42095</v>
+      </c>
+      <c r="J7" s="13">
+        <v>42095</v>
+      </c>
+      <c r="K7" s="13">
+        <v>42095</v>
+      </c>
+      <c r="L7" s="9"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="18"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B8" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="16"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A8" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="9"/>
+      <c r="E8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="13"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="16"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="L8" s="9"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="18"/>
+    </row>
+    <row r="9" spans="1:16" ht="24" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>62</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C9" s="11"/>
       <c r="D9" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="13"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="16"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="L9" s="15">
+        <v>42101</v>
+      </c>
+      <c r="M9" s="17"/>
+      <c r="N9" s="18"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="13">
+        <v>42095</v>
+      </c>
+      <c r="J10" s="13">
+        <v>42095</v>
+      </c>
+      <c r="K10" s="13">
+        <v>42095</v>
+      </c>
+      <c r="L10" s="13">
+        <v>42095</v>
+      </c>
+      <c r="M10" s="17"/>
+      <c r="N10" s="18"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B11" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="16"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A11" s="10" t="s">
+      <c r="C11" s="11"/>
+      <c r="D11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="13">
+        <v>42095</v>
+      </c>
+      <c r="J11" s="13">
+        <v>42095</v>
+      </c>
+      <c r="K11" s="13">
+        <v>42095</v>
+      </c>
+      <c r="L11" s="13">
+        <v>42095</v>
+      </c>
+      <c r="M11" s="17"/>
+      <c r="N11" s="18"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B12" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="16"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A12" s="10" t="s">
+      <c r="C12" s="11"/>
+      <c r="D12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="13">
+        <v>42095</v>
+      </c>
+      <c r="J12" s="13">
+        <v>42095</v>
+      </c>
+      <c r="K12" s="13">
+        <v>42095</v>
+      </c>
+      <c r="L12" s="13">
+        <v>42095</v>
+      </c>
+      <c r="M12" s="17"/>
+      <c r="N12" s="18"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B13" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="8" t="s">
+      <c r="C13" s="11"/>
+      <c r="D13" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="16"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A13" s="10" t="s">
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="13">
+        <v>42100</v>
+      </c>
+      <c r="J13" s="13">
+        <v>42100</v>
+      </c>
+      <c r="K13" s="13">
+        <v>42100</v>
+      </c>
+      <c r="L13" s="9"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="18"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B14" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="16"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A14" s="10" t="s">
+      <c r="C14" s="11"/>
+      <c r="D14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="13">
+        <v>42101</v>
+      </c>
+      <c r="J14" s="15">
+        <v>42101</v>
+      </c>
+      <c r="K14" s="15">
+        <v>42101</v>
+      </c>
+      <c r="L14" s="13">
+        <v>42101</v>
+      </c>
+      <c r="M14" s="17"/>
+      <c r="N14" s="18"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B15" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="8" t="s">
+      <c r="C15" s="11"/>
+      <c r="D15" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="16"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A15" s="10" t="s">
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="13">
+        <v>42101</v>
+      </c>
+      <c r="J15" s="13">
+        <v>42101</v>
+      </c>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="18"/>
+    </row>
+    <row r="16" spans="1:16" ht="24" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B16" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="16"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A16" s="10" t="s">
+      <c r="C16" s="11"/>
+      <c r="D16" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="13">
+        <v>42101</v>
+      </c>
+      <c r="J16" s="13">
+        <v>42101</v>
+      </c>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="18"/>
+    </row>
+    <row r="17" spans="1:14" ht="24" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B17" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="16"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A17" s="10" t="s">
+      <c r="C17" s="11"/>
+      <c r="D17" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="13">
+        <v>42101</v>
+      </c>
+      <c r="J17" s="13">
+        <v>42101</v>
+      </c>
+      <c r="K17" s="13">
+        <v>42101</v>
+      </c>
+      <c r="L17" s="13">
+        <v>42101</v>
+      </c>
+      <c r="M17" s="17"/>
+      <c r="N17" s="18"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B18" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="16"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A18" s="10" t="s">
+      <c r="C18" s="11"/>
+      <c r="D18" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="13">
+        <v>42101</v>
+      </c>
+      <c r="J18" s="13">
+        <v>42101</v>
+      </c>
+      <c r="K18" s="13">
+        <v>42101</v>
+      </c>
+      <c r="L18" s="13">
+        <v>42101</v>
+      </c>
+      <c r="M18" s="17"/>
+      <c r="N18" s="18"/>
+    </row>
+    <row r="19" spans="1:14" ht="24" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B19" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="8" t="s">
+      <c r="C19" s="11"/>
+      <c r="D19" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="16"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A19" s="10" t="s">
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="13">
+        <v>42101</v>
+      </c>
+      <c r="J19" s="13">
+        <v>42101</v>
+      </c>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="18"/>
+    </row>
+    <row r="20" spans="1:14" ht="24" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B20" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="16"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A20" s="10" t="s">
+      <c r="C20" s="11"/>
+      <c r="D20" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="13">
+        <v>42101</v>
+      </c>
+      <c r="J20" s="13">
+        <v>42101</v>
+      </c>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="18"/>
+    </row>
+    <row r="21" spans="1:14" ht="24" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B21" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="16"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A21" s="10" t="s">
+      <c r="C21" s="11"/>
+      <c r="D21" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="13">
+        <v>42101</v>
+      </c>
+      <c r="J21" s="13">
+        <v>42101</v>
+      </c>
+      <c r="K21" s="13">
+        <v>42101</v>
+      </c>
+      <c r="L21" s="13">
+        <v>42101</v>
+      </c>
+      <c r="M21" s="17"/>
+      <c r="N21" s="18"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B22" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="16"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A22" s="10" t="s">
+      <c r="C22" s="11"/>
+      <c r="D22" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="13">
+        <v>42101</v>
+      </c>
+      <c r="J22" s="13">
+        <v>42101</v>
+      </c>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="18"/>
+    </row>
+    <row r="23" spans="1:14" ht="24" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B23" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="16"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A23" s="10" t="s">
+      <c r="C23" s="11"/>
+      <c r="D23" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="13">
+        <v>42101</v>
+      </c>
+      <c r="J23" s="13">
+        <v>42101</v>
+      </c>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="18"/>
+    </row>
+    <row r="24" spans="1:14" ht="24" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B24" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="16"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A24" s="10" t="s">
+      <c r="C24" s="11"/>
+      <c r="D24" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="13">
+        <v>42101</v>
+      </c>
+      <c r="J24" s="13">
+        <v>42101</v>
+      </c>
+      <c r="K24" s="13">
+        <v>42101</v>
+      </c>
+      <c r="L24" s="13">
+        <v>42101</v>
+      </c>
+      <c r="M24" s="17"/>
+      <c r="N24" s="18"/>
+    </row>
+    <row r="25" spans="1:14" ht="24" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B25" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="16"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A25" s="10" t="s">
+      <c r="C25" s="11"/>
+      <c r="D25" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="13">
+        <v>42101</v>
+      </c>
+      <c r="J25" s="13">
+        <v>42101</v>
+      </c>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="18"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B26" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="16"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A26" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>62</v>
-      </c>
+      <c r="C26" s="11"/>
       <c r="D26" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="13"/>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="16"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="18"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="L4:L26"/>
-    <mergeCell ref="M4:M26"/>
-    <mergeCell ref="E4:E26"/>
-    <mergeCell ref="F4:F26"/>
-    <mergeCell ref="G4:G26"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="M5:M27"/>
+    <mergeCell ref="N5:N27"/>
+    <mergeCell ref="F5:F27"/>
+    <mergeCell ref="G5:G27"/>
+    <mergeCell ref="H5:H27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>